<commit_message>
Corrected errors in transportation variables and coordinated fuel economy variables
</commit_message>
<xml_diff>
--- a/InputData/trans/AVL/Avg Vehicle Lifetime.xlsx
+++ b/InputData/trans/AVL/Avg Vehicle Lifetime.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipL\InputData\trans\AVL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-brazil\InputData\trans\AVL\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1460,9 +1460,24 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="27" xfId="58" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="58" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="22" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1471,21 +1486,6 @@
     </xf>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="27" xfId="58" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="58" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="22" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="62">
@@ -2165,62 +2165,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:54" s="13" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="89" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="91"/>
-      <c r="C1" s="91"/>
-      <c r="D1" s="91"/>
-      <c r="E1" s="91"/>
-      <c r="F1" s="91"/>
-      <c r="G1" s="91"/>
-      <c r="H1" s="91"/>
-      <c r="I1" s="91"/>
-      <c r="J1" s="91"/>
-      <c r="K1" s="91"/>
-      <c r="L1" s="91"/>
-      <c r="M1" s="91"/>
-      <c r="N1" s="91"/>
-      <c r="O1" s="91"/>
-      <c r="P1" s="91"/>
-      <c r="Q1" s="91"/>
-      <c r="R1" s="91"/>
-      <c r="S1" s="91"/>
-      <c r="T1" s="91"/>
-      <c r="U1" s="91"/>
-      <c r="V1" s="91"/>
-      <c r="W1" s="91"/>
-      <c r="X1" s="91"/>
-      <c r="Y1" s="91"/>
-      <c r="Z1" s="91"/>
-      <c r="AA1" s="91"/>
-      <c r="AB1" s="91"/>
-      <c r="AC1" s="92"/>
-      <c r="AD1" s="92"/>
-      <c r="AE1" s="92"/>
-      <c r="AF1" s="92"/>
-      <c r="AG1" s="92"/>
-      <c r="AH1" s="92"/>
-      <c r="AI1" s="92"/>
-      <c r="AJ1" s="92"/>
-      <c r="AK1" s="92"/>
-      <c r="AL1" s="92"/>
-      <c r="AM1" s="92"/>
-      <c r="AN1" s="92"/>
-      <c r="AO1" s="92"/>
-      <c r="AP1" s="92"/>
-      <c r="AQ1" s="92"/>
-      <c r="AR1" s="92"/>
-      <c r="AS1" s="92"/>
-      <c r="AT1" s="92"/>
-      <c r="AU1" s="92"/>
-      <c r="AV1" s="92"/>
-      <c r="AW1" s="92"/>
-      <c r="AX1" s="92"/>
-      <c r="AY1" s="92"/>
-      <c r="AZ1" s="92"/>
-      <c r="BA1" s="92"/>
-      <c r="BB1" s="92"/>
+      <c r="B1" s="89"/>
+      <c r="C1" s="89"/>
+      <c r="D1" s="89"/>
+      <c r="E1" s="89"/>
+      <c r="F1" s="89"/>
+      <c r="G1" s="89"/>
+      <c r="H1" s="89"/>
+      <c r="I1" s="89"/>
+      <c r="J1" s="89"/>
+      <c r="K1" s="89"/>
+      <c r="L1" s="89"/>
+      <c r="M1" s="89"/>
+      <c r="N1" s="89"/>
+      <c r="O1" s="89"/>
+      <c r="P1" s="89"/>
+      <c r="Q1" s="89"/>
+      <c r="R1" s="89"/>
+      <c r="S1" s="89"/>
+      <c r="T1" s="89"/>
+      <c r="U1" s="89"/>
+      <c r="V1" s="89"/>
+      <c r="W1" s="89"/>
+      <c r="X1" s="89"/>
+      <c r="Y1" s="89"/>
+      <c r="Z1" s="89"/>
+      <c r="AA1" s="89"/>
+      <c r="AB1" s="89"/>
+      <c r="AC1" s="90"/>
+      <c r="AD1" s="90"/>
+      <c r="AE1" s="90"/>
+      <c r="AF1" s="90"/>
+      <c r="AG1" s="90"/>
+      <c r="AH1" s="90"/>
+      <c r="AI1" s="90"/>
+      <c r="AJ1" s="90"/>
+      <c r="AK1" s="90"/>
+      <c r="AL1" s="90"/>
+      <c r="AM1" s="90"/>
+      <c r="AN1" s="90"/>
+      <c r="AO1" s="90"/>
+      <c r="AP1" s="90"/>
+      <c r="AQ1" s="90"/>
+      <c r="AR1" s="90"/>
+      <c r="AS1" s="90"/>
+      <c r="AT1" s="90"/>
+      <c r="AU1" s="90"/>
+      <c r="AV1" s="90"/>
+      <c r="AW1" s="90"/>
+      <c r="AX1" s="90"/>
+      <c r="AY1" s="90"/>
+      <c r="AZ1" s="90"/>
+      <c r="BA1" s="90"/>
+      <c r="BB1" s="90"/>
     </row>
     <row r="2" spans="1:54" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="46"/>
@@ -4243,189 +4243,189 @@
       <c r="BB20" s="72"/>
     </row>
     <row r="21" spans="1:54" s="76" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="93" t="s">
+      <c r="A21" s="91" t="s">
         <v>74</v>
       </c>
-      <c r="B21" s="93"/>
-      <c r="C21" s="93"/>
-      <c r="D21" s="93"/>
-      <c r="E21" s="93"/>
-      <c r="F21" s="93"/>
-      <c r="G21" s="93"/>
-      <c r="H21" s="93"/>
-      <c r="I21" s="93"/>
-      <c r="J21" s="93"/>
-      <c r="K21" s="93"/>
-      <c r="L21" s="93"/>
-      <c r="M21" s="93"/>
-      <c r="N21" s="93"/>
-      <c r="O21" s="93"/>
-      <c r="P21" s="93"/>
-      <c r="Q21" s="93"/>
+      <c r="B21" s="91"/>
+      <c r="C21" s="91"/>
+      <c r="D21" s="91"/>
+      <c r="E21" s="91"/>
+      <c r="F21" s="91"/>
+      <c r="G21" s="91"/>
+      <c r="H21" s="91"/>
+      <c r="I21" s="91"/>
+      <c r="J21" s="91"/>
+      <c r="K21" s="91"/>
+      <c r="L21" s="91"/>
+      <c r="M21" s="91"/>
+      <c r="N21" s="91"/>
+      <c r="O21" s="91"/>
+      <c r="P21" s="91"/>
+      <c r="Q21" s="91"/>
     </row>
     <row r="22" spans="1:54" s="76" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="94"/>
-      <c r="B22" s="94"/>
-      <c r="C22" s="94"/>
-      <c r="D22" s="94"/>
-      <c r="E22" s="94"/>
-      <c r="F22" s="94"/>
-      <c r="G22" s="94"/>
-      <c r="H22" s="94"/>
-      <c r="I22" s="94"/>
-      <c r="J22" s="94"/>
-      <c r="K22" s="94"/>
-      <c r="L22" s="94"/>
-      <c r="M22" s="94"/>
-      <c r="N22" s="94"/>
-      <c r="O22" s="94"/>
-      <c r="P22" s="94"/>
-      <c r="Q22" s="94"/>
+      <c r="A22" s="92"/>
+      <c r="B22" s="92"/>
+      <c r="C22" s="92"/>
+      <c r="D22" s="92"/>
+      <c r="E22" s="92"/>
+      <c r="F22" s="92"/>
+      <c r="G22" s="92"/>
+      <c r="H22" s="92"/>
+      <c r="I22" s="92"/>
+      <c r="J22" s="92"/>
+      <c r="K22" s="92"/>
+      <c r="L22" s="92"/>
+      <c r="M22" s="92"/>
+      <c r="N22" s="92"/>
+      <c r="O22" s="92"/>
+      <c r="P22" s="92"/>
+      <c r="Q22" s="92"/>
     </row>
     <row r="23" spans="1:54" s="76" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="94" t="s">
+      <c r="A23" s="92" t="s">
         <v>75</v>
       </c>
-      <c r="B23" s="94"/>
-      <c r="C23" s="94"/>
-      <c r="D23" s="94"/>
-      <c r="E23" s="94"/>
-      <c r="F23" s="94"/>
-      <c r="G23" s="94"/>
-      <c r="H23" s="94"/>
-      <c r="I23" s="94"/>
-      <c r="J23" s="94"/>
-      <c r="K23" s="94"/>
-      <c r="L23" s="94"/>
-      <c r="M23" s="94"/>
-      <c r="N23" s="94"/>
-      <c r="O23" s="94"/>
-      <c r="P23" s="94"/>
-      <c r="Q23" s="94"/>
+      <c r="B23" s="92"/>
+      <c r="C23" s="92"/>
+      <c r="D23" s="92"/>
+      <c r="E23" s="92"/>
+      <c r="F23" s="92"/>
+      <c r="G23" s="92"/>
+      <c r="H23" s="92"/>
+      <c r="I23" s="92"/>
+      <c r="J23" s="92"/>
+      <c r="K23" s="92"/>
+      <c r="L23" s="92"/>
+      <c r="M23" s="92"/>
+      <c r="N23" s="92"/>
+      <c r="O23" s="92"/>
+      <c r="P23" s="92"/>
+      <c r="Q23" s="92"/>
     </row>
     <row r="24" spans="1:54" s="76" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="87" t="s">
+      <c r="A24" s="88" t="s">
         <v>76</v>
       </c>
-      <c r="B24" s="87"/>
-      <c r="C24" s="87"/>
-      <c r="D24" s="87"/>
-      <c r="E24" s="87"/>
-      <c r="F24" s="87"/>
-      <c r="G24" s="87"/>
-      <c r="H24" s="87"/>
-      <c r="I24" s="87"/>
-      <c r="J24" s="87"/>
-      <c r="K24" s="87"/>
-      <c r="L24" s="87"/>
-      <c r="M24" s="87"/>
-      <c r="N24" s="87"/>
-      <c r="O24" s="87"/>
-      <c r="P24" s="87"/>
-      <c r="Q24" s="87"/>
+      <c r="B24" s="88"/>
+      <c r="C24" s="88"/>
+      <c r="D24" s="88"/>
+      <c r="E24" s="88"/>
+      <c r="F24" s="88"/>
+      <c r="G24" s="88"/>
+      <c r="H24" s="88"/>
+      <c r="I24" s="88"/>
+      <c r="J24" s="88"/>
+      <c r="K24" s="88"/>
+      <c r="L24" s="88"/>
+      <c r="M24" s="88"/>
+      <c r="N24" s="88"/>
+      <c r="O24" s="88"/>
+      <c r="P24" s="88"/>
+      <c r="Q24" s="88"/>
     </row>
     <row r="25" spans="1:54" s="76" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="87" t="s">
+      <c r="A25" s="88" t="s">
         <v>77</v>
       </c>
-      <c r="B25" s="87"/>
-      <c r="C25" s="87"/>
-      <c r="D25" s="87"/>
-      <c r="E25" s="87"/>
-      <c r="F25" s="87"/>
-      <c r="G25" s="87"/>
-      <c r="H25" s="87"/>
-      <c r="I25" s="87"/>
-      <c r="J25" s="87"/>
-      <c r="K25" s="87"/>
-      <c r="L25" s="87"/>
-      <c r="M25" s="87"/>
-      <c r="N25" s="87"/>
-      <c r="O25" s="87"/>
-      <c r="P25" s="87"/>
-      <c r="Q25" s="87"/>
+      <c r="B25" s="88"/>
+      <c r="C25" s="88"/>
+      <c r="D25" s="88"/>
+      <c r="E25" s="88"/>
+      <c r="F25" s="88"/>
+      <c r="G25" s="88"/>
+      <c r="H25" s="88"/>
+      <c r="I25" s="88"/>
+      <c r="J25" s="88"/>
+      <c r="K25" s="88"/>
+      <c r="L25" s="88"/>
+      <c r="M25" s="88"/>
+      <c r="N25" s="88"/>
+      <c r="O25" s="88"/>
+      <c r="P25" s="88"/>
+      <c r="Q25" s="88"/>
     </row>
     <row r="26" spans="1:54" s="76" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="88" t="s">
+      <c r="A26" s="93" t="s">
         <v>78</v>
       </c>
-      <c r="B26" s="88"/>
-      <c r="C26" s="88"/>
-      <c r="D26" s="88"/>
-      <c r="E26" s="88"/>
-      <c r="F26" s="88"/>
-      <c r="G26" s="88"/>
-      <c r="H26" s="88"/>
-      <c r="I26" s="88"/>
-      <c r="J26" s="88"/>
-      <c r="K26" s="88"/>
-      <c r="L26" s="88"/>
-      <c r="M26" s="88"/>
-      <c r="N26" s="88"/>
-      <c r="O26" s="88"/>
-      <c r="P26" s="88"/>
-      <c r="Q26" s="88"/>
+      <c r="B26" s="93"/>
+      <c r="C26" s="93"/>
+      <c r="D26" s="93"/>
+      <c r="E26" s="93"/>
+      <c r="F26" s="93"/>
+      <c r="G26" s="93"/>
+      <c r="H26" s="93"/>
+      <c r="I26" s="93"/>
+      <c r="J26" s="93"/>
+      <c r="K26" s="93"/>
+      <c r="L26" s="93"/>
+      <c r="M26" s="93"/>
+      <c r="N26" s="93"/>
+      <c r="O26" s="93"/>
+      <c r="P26" s="93"/>
+      <c r="Q26" s="93"/>
     </row>
     <row r="27" spans="1:54" s="76" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A27" s="88"/>
-      <c r="B27" s="88"/>
-      <c r="C27" s="88"/>
-      <c r="D27" s="88"/>
-      <c r="E27" s="88"/>
-      <c r="F27" s="88"/>
-      <c r="G27" s="88"/>
-      <c r="H27" s="88"/>
-      <c r="I27" s="88"/>
-      <c r="J27" s="88"/>
-      <c r="K27" s="88"/>
-      <c r="L27" s="88"/>
-      <c r="M27" s="88"/>
-      <c r="N27" s="88"/>
-      <c r="O27" s="88"/>
-      <c r="P27" s="88"/>
-      <c r="Q27" s="88"/>
+      <c r="A27" s="93"/>
+      <c r="B27" s="93"/>
+      <c r="C27" s="93"/>
+      <c r="D27" s="93"/>
+      <c r="E27" s="93"/>
+      <c r="F27" s="93"/>
+      <c r="G27" s="93"/>
+      <c r="H27" s="93"/>
+      <c r="I27" s="93"/>
+      <c r="J27" s="93"/>
+      <c r="K27" s="93"/>
+      <c r="L27" s="93"/>
+      <c r="M27" s="93"/>
+      <c r="N27" s="93"/>
+      <c r="O27" s="93"/>
+      <c r="P27" s="93"/>
+      <c r="Q27" s="93"/>
     </row>
     <row r="28" spans="1:54" s="76" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="89" t="s">
+      <c r="A28" s="94" t="s">
         <v>79</v>
       </c>
-      <c r="B28" s="89"/>
-      <c r="C28" s="89"/>
-      <c r="D28" s="89"/>
-      <c r="E28" s="89"/>
-      <c r="F28" s="89"/>
-      <c r="G28" s="89"/>
-      <c r="H28" s="89"/>
-      <c r="I28" s="89"/>
-      <c r="J28" s="89"/>
-      <c r="K28" s="89"/>
-      <c r="L28" s="89"/>
-      <c r="M28" s="89"/>
-      <c r="N28" s="89"/>
-      <c r="O28" s="89"/>
-      <c r="P28" s="89"/>
-      <c r="Q28" s="89"/>
+      <c r="B28" s="94"/>
+      <c r="C28" s="94"/>
+      <c r="D28" s="94"/>
+      <c r="E28" s="94"/>
+      <c r="F28" s="94"/>
+      <c r="G28" s="94"/>
+      <c r="H28" s="94"/>
+      <c r="I28" s="94"/>
+      <c r="J28" s="94"/>
+      <c r="K28" s="94"/>
+      <c r="L28" s="94"/>
+      <c r="M28" s="94"/>
+      <c r="N28" s="94"/>
+      <c r="O28" s="94"/>
+      <c r="P28" s="94"/>
+      <c r="Q28" s="94"/>
     </row>
     <row r="29" spans="1:54" s="76" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="90" t="s">
+      <c r="A29" s="95" t="s">
         <v>80</v>
       </c>
-      <c r="B29" s="90"/>
-      <c r="C29" s="90"/>
-      <c r="D29" s="90"/>
-      <c r="E29" s="90"/>
-      <c r="F29" s="90"/>
-      <c r="G29" s="90"/>
-      <c r="H29" s="90"/>
-      <c r="I29" s="90"/>
-      <c r="J29" s="90"/>
-      <c r="K29" s="90"/>
-      <c r="L29" s="90"/>
-      <c r="M29" s="90"/>
-      <c r="N29" s="90"/>
-      <c r="O29" s="90"/>
-      <c r="P29" s="90"/>
-      <c r="Q29" s="90"/>
+      <c r="B29" s="95"/>
+      <c r="C29" s="95"/>
+      <c r="D29" s="95"/>
+      <c r="E29" s="95"/>
+      <c r="F29" s="95"/>
+      <c r="G29" s="95"/>
+      <c r="H29" s="95"/>
+      <c r="I29" s="95"/>
+      <c r="J29" s="95"/>
+      <c r="K29" s="95"/>
+      <c r="L29" s="95"/>
+      <c r="M29" s="95"/>
+      <c r="N29" s="95"/>
+      <c r="O29" s="95"/>
+      <c r="P29" s="95"/>
+      <c r="Q29" s="95"/>
     </row>
     <row r="30" spans="1:54" s="77" customFormat="1" x14ac:dyDescent="0.45"/>
     <row r="31" spans="1:54" s="77" customFormat="1" x14ac:dyDescent="0.45"/>
@@ -4461,17 +4461,17 @@
     <row r="61" s="77" customFormat="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A25:Q25"/>
+    <mergeCell ref="A26:Q26"/>
+    <mergeCell ref="A27:Q27"/>
+    <mergeCell ref="A28:Q28"/>
+    <mergeCell ref="A29:Q29"/>
     <mergeCell ref="A24:Q24"/>
     <mergeCell ref="A1:AB1"/>
     <mergeCell ref="AC1:BB1"/>
     <mergeCell ref="A21:Q21"/>
     <mergeCell ref="A22:Q22"/>
     <mergeCell ref="A23:Q23"/>
-    <mergeCell ref="A25:Q25"/>
-    <mergeCell ref="A26:Q26"/>
-    <mergeCell ref="A27:Q27"/>
-    <mergeCell ref="A28:Q28"/>
-    <mergeCell ref="A29:Q29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5025,7 +5025,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="95" t="s">
+      <c r="A1" s="87" t="s">
         <v>100</v>
       </c>
       <c r="B1" s="11" t="s">

</xml_diff>